<commit_message>
added in the results from the altered dataset
</commit_message>
<xml_diff>
--- a/Analysis/Tables.xlsx
+++ b/Analysis/Tables.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="17235" windowHeight="4935" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="17235" windowHeight="4935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="2" r:id="rId1"/>
     <sheet name="Table2" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Model</t>
   </si>
@@ -44,12 +45,6 @@
     <t>0.1 (0, 0.3)</t>
   </si>
   <si>
-    <t>1.5 (0.1, 4.8)</t>
-  </si>
-  <si>
-    <t>5.7 (1.5, 14)</t>
-  </si>
-  <si>
     <t>February</t>
   </si>
   <si>
@@ -65,33 +60,9 @@
     <t>April</t>
   </si>
   <si>
-    <t>1.0 (0.1, 3.4)</t>
-  </si>
-  <si>
-    <t>1.0 (0.1, 3.5)</t>
-  </si>
-  <si>
-    <t>5.8 (2.3, 11)</t>
-  </si>
-  <si>
-    <t>5.8 (2.2, 12)</t>
-  </si>
-  <si>
     <t>5.4 (1.5, 13)</t>
   </si>
   <si>
-    <t>4.7 (1.8, 9)</t>
-  </si>
-  <si>
-    <t>4.6 (1.9, 9)</t>
-  </si>
-  <si>
-    <t>5 (1.4, 12)</t>
-  </si>
-  <si>
-    <t>5.9 (1.9, 12)</t>
-  </si>
-  <si>
     <t>5.7 (1.9, 12)</t>
   </si>
   <si>
@@ -99,12 +70,60 @@
   </si>
   <si>
     <t>1.0 (0.2, 2.6)</t>
+  </si>
+  <si>
+    <t>1.5 (0.2, 4.9)</t>
+  </si>
+  <si>
+    <t>1.0 (0.1, 3.3)</t>
+  </si>
+  <si>
+    <t>5.4 (2.0, 11)</t>
+  </si>
+  <si>
+    <t>5.3 (2.1, 11)</t>
+  </si>
+  <si>
+    <t>5.0 (1.3, 12)</t>
+  </si>
+  <si>
+    <t>5.0 (2.0, 10)</t>
+  </si>
+  <si>
+    <t>4.8 (2.1, 8.7)</t>
+  </si>
+  <si>
+    <t>5.3 (1.7, 11)</t>
+  </si>
+  <si>
+    <t>5.5 (1.5, 14)</t>
+  </si>
+  <si>
+    <t>1.0 (0.2, 2.7)</t>
+  </si>
+  <si>
+    <t>Table 1b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event </t>
+  </si>
+  <si>
+    <t>Abortion</t>
+  </si>
+  <si>
+    <t>Birth</t>
+  </si>
+  <si>
+    <t>Seropositive only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -605,7 +624,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -627,6 +646,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -974,7 +1008,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1020,13 +1054,13 @@
         <v>41695</v>
       </c>
       <c r="E2" s="8">
-        <v>41718</v>
+        <v>41719</v>
       </c>
       <c r="F2" s="8">
         <v>41768</v>
       </c>
       <c r="G2" s="8">
-        <v>41793</v>
+        <v>41794</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1040,7 +1074,7 @@
         <v>16.3</v>
       </c>
       <c r="D3" s="8">
-        <v>41695</v>
+        <v>41694</v>
       </c>
       <c r="E3" s="8">
         <v>41718</v>
@@ -1063,7 +1097,7 @@
         <v>22.6</v>
       </c>
       <c r="D4" s="9">
-        <v>41664</v>
+        <v>41663</v>
       </c>
       <c r="E4" s="9">
         <v>41713</v>
@@ -1089,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,22 +1138,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1127,19 +1161,19 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>7</v>
@@ -1150,22 +1184,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1173,16 +1207,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>27</v>
@@ -1194,4 +1228,252 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="3" width="7.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1027.0999999999999</v>
+      </c>
+      <c r="C4" s="7">
+        <v>12.2</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="14">
+        <v>41695</v>
+      </c>
+      <c r="F5" s="14">
+        <v>41719</v>
+      </c>
+      <c r="G5" s="14">
+        <v>41768</v>
+      </c>
+      <c r="H5" s="14">
+        <v>41794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="14">
+        <v>41779</v>
+      </c>
+      <c r="F7" s="14">
+        <v>41787</v>
+      </c>
+      <c r="G7" s="14">
+        <v>41800</v>
+      </c>
+      <c r="H7" s="14">
+        <v>41814</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1025.7</v>
+      </c>
+      <c r="C9" s="7">
+        <v>16.3</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="14">
+        <v>41694</v>
+      </c>
+      <c r="F10" s="14">
+        <v>41718</v>
+      </c>
+      <c r="G10" s="14">
+        <v>41767</v>
+      </c>
+      <c r="H10" s="14">
+        <v>41793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="14">
+        <v>41779</v>
+      </c>
+      <c r="F12" s="14">
+        <v>41787</v>
+      </c>
+      <c r="G12" s="14">
+        <v>41800</v>
+      </c>
+      <c r="H12" s="14">
+        <v>41815</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="12">
+        <v>1026.9000000000001</v>
+      </c>
+      <c r="C14" s="12">
+        <v>22.6</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="15">
+        <v>41663</v>
+      </c>
+      <c r="F15" s="15">
+        <v>41713</v>
+      </c>
+      <c r="G15" s="15">
+        <v>41765</v>
+      </c>
+      <c r="H15" s="15">
+        <v>41792</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="17">
+        <v>41780</v>
+      </c>
+      <c r="F17" s="17">
+        <v>41787</v>
+      </c>
+      <c r="G17" s="17">
+        <v>41799</v>
+      </c>
+      <c r="H17" s="17">
+        <v>41814</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mostly done with the reviewer comments edits...just a few odds and ends.
</commit_message>
<xml_diff>
--- a/Analysis/Tables.xlsx
+++ b/Analysis/Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="17235" windowHeight="4935" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="17235" windowHeight="4935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="2" r:id="rId1"/>
@@ -122,7 +122,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -653,14 +653,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>